<commit_message>
Sanity test scenario for Neev
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2662-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-AccCL1stFEB-PREPAY-ON-2ndFEB-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/2662-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-AccCL1stFEB-PREPAY-ON-2ndFEB-Newcreateloan1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -171,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -278,6 +283,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -325,7 +333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,9 +366,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,6 +418,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -820,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -976,14 +1018,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>